<commit_message>
Starting a try in heroku
</commit_message>
<xml_diff>
--- a/data/coffee.xlsx
+++ b/data/coffee.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7100" uniqueCount="6876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7115" uniqueCount="6891">
   <si>
     <t xml:space="preserve">Café | INDICADOR DO CAFÉ ARÁBICA CEPEA/ESALQ</t>
   </si>
@@ -20649,6 +20649,51 @@
   </si>
   <si>
     <t xml:space="preserve">346,42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/06/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.877,02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">342,15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/06/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.834,36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">337,82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/07/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.807,41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330,85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/07/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.779,95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">328,16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/07/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.742,20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">321,91</t>
   </si>
 </sst>
 </file>
@@ -20795,7 +20840,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2368"/>
+  <dimension ref="A1:J2373"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -46867,6 +46912,61 @@
       </c>
       <c r="C2368" s="6" t="s">
         <v>6875</v>
+      </c>
+    </row>
+    <row r="2369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2369" s="6" t="s">
+        <v>6876</v>
+      </c>
+      <c r="B2369" s="6" t="s">
+        <v>6877</v>
+      </c>
+      <c r="C2369" s="6" t="s">
+        <v>6878</v>
+      </c>
+    </row>
+    <row r="2370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2370" s="6" t="s">
+        <v>6879</v>
+      </c>
+      <c r="B2370" s="6" t="s">
+        <v>6880</v>
+      </c>
+      <c r="C2370" s="6" t="s">
+        <v>6881</v>
+      </c>
+    </row>
+    <row r="2371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2371" s="6" t="s">
+        <v>6882</v>
+      </c>
+      <c r="B2371" s="6" t="s">
+        <v>6883</v>
+      </c>
+      <c r="C2371" s="6" t="s">
+        <v>6884</v>
+      </c>
+    </row>
+    <row r="2372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2372" s="6" t="s">
+        <v>6885</v>
+      </c>
+      <c r="B2372" s="6" t="s">
+        <v>6886</v>
+      </c>
+      <c r="C2372" s="6" t="s">
+        <v>6887</v>
+      </c>
+    </row>
+    <row r="2373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2373" s="6" t="s">
+        <v>6888</v>
+      </c>
+      <c r="B2373" s="6" t="s">
+        <v>6889</v>
+      </c>
+      <c r="C2373" s="6" t="s">
+        <v>6890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>